<commit_message>
Xóa các tệp JSON không còn cần thiết và cập nhật đường dẫn cho các tệp JSON trong mã nguồn. Cập nhật quy trình chuyển đổi từ Excel sang JSON trong excel2json_model.py.
</commit_message>
<xml_diff>
--- a/Bike Chooser _ Honda Powersports - Street.xlsx
+++ b/Bike Chooser _ Honda Powersports - Street.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dat.ta/Desktop/code/work/honda-help-me-choose-automate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18545AA-D78D-E346-A420-97763B111966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C4CC16-3C03-944D-8BFC-FA7F7881D454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40960" yWindow="0" windowWidth="40960" windowHeight="23040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40960" yWindow="500" windowWidth="40960" windowHeight="22540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUESTIONS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="218">
   <si>
     <t>Question</t>
   </si>
@@ -481,9 +481,6 @@
     <t>REC/UTLITY ATV</t>
   </si>
   <si>
-    <t>03 Use DESERT/DUNES</t>
-  </si>
-  <si>
     <t xml:space="preserve">FourTrax Rubicon 700 </t>
   </si>
   <si>
@@ -502,6 +499,45 @@
     <t>SPORT ATV</t>
   </si>
   <si>
+    <t>MOSTLY WORK</t>
+  </si>
+  <si>
+    <t>MIX WORK &amp; REC.</t>
+  </si>
+  <si>
+    <t>MOSTLY REC.</t>
+  </si>
+  <si>
+    <t>FUN/CASUAL RIDING</t>
+  </si>
+  <si>
+    <t>FARMING/RANCHING</t>
+  </si>
+  <si>
+    <t>GENERAL MAINT.</t>
+  </si>
+  <si>
+    <t>PLOWING SNOW</t>
+  </si>
+  <si>
+    <t>HUNTING/FISHING</t>
+  </si>
+  <si>
+    <t>TRAIL RIDING</t>
+  </si>
+  <si>
+    <t>DESERT/DUNES</t>
+  </si>
+  <si>
+    <t>LIGHT/MODERATE</t>
+  </si>
+  <si>
+    <t>MEDIUM/BALANCED</t>
+  </si>
+  <si>
+    <t>HIGH/HEAVY DUTY</t>
+  </si>
+  <si>
     <t>TRX250X</t>
   </si>
   <si>
@@ -536,6 +572,21 @@
   </si>
   <si>
     <t>SPORT SxS</t>
+  </si>
+  <si>
+    <t>RACING/HIGH PERF.</t>
+  </si>
+  <si>
+    <t>MUDDING/ROCK CRAWLING</t>
+  </si>
+  <si>
+    <t>ME PLUS ONE</t>
+  </si>
+  <si>
+    <t>UP TO FOUR</t>
+  </si>
+  <si>
+    <t>UP TO SIX</t>
   </si>
   <si>
     <t>Talon 1000R-4 FOX LIVE VALVE</t>
@@ -669,7 +720,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -716,6 +767,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -810,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1014,9 +1072,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1081,6 +1136,9 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1098,17 +1156,9 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1486,8 +1536,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table_12" displayName="Table_12" ref="A7:Z11" headerRowCount="0">
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table_12" displayName="Table_12" ref="A7:Y11" headerRowCount="0">
+  <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Column2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Column3"/>
@@ -1502,7 +1552,6 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0B00-00000C000000}" name="Column12"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0B00-00000D000000}" name="Column13"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0B00-00000E000000}" name="Column14"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0B00-00000F000000}" name="Column15"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0B00-000010000000}" name="Column16"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0B00-000011000000}" name="Column17"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0B00-000012000000}" name="Column18"/>
@@ -1520,7 +1569,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table_13" displayName="Table_13" ref="A6:AA18" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table_13" displayName="Table_13" ref="A6:AA19" headerRowCount="0">
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Column2"/>
@@ -2120,7 +2169,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B15" sqref="B15:J15"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2203,7 +2252,7 @@
       <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -2229,7 +2278,7 @@
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="85"/>
+      <c r="C4" s="84"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -2271,9 +2320,9 @@
     <row r="6" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="84" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="83" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -2299,9 +2348,9 @@
     <row r="7" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="85" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="49" t="s">
@@ -2319,10 +2368,10 @@
       <c r="H7" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="87" t="s">
+      <c r="I7" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="87" t="s">
+      <c r="J7" s="86" t="s">
         <v>24</v>
       </c>
       <c r="K7" s="49"/>
@@ -2337,9 +2386,9 @@
     <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="88" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="87" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -2354,7 +2403,7 @@
       <c r="G8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="89"/>
+      <c r="H8" s="88"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
@@ -2369,9 +2418,9 @@
     <row r="9" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="16"/>
       <c r="B9" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" s="86" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="85" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="49" t="s">
@@ -2397,9 +2446,9 @@
     <row r="10" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="18"/>
       <c r="B10" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="88" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="87" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="21" t="s">
@@ -2425,7 +2474,7 @@
     <row r="11" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>36</v>
@@ -2438,7 +2487,7 @@
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="87"/>
+      <c r="H11" s="86"/>
       <c r="I11" s="49"/>
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
@@ -2479,7 +2528,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="90"/>
+      <c r="G13" s="89"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
@@ -2495,7 +2544,7 @@
     <row r="14" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>40</v>
@@ -2523,7 +2572,7 @@
     <row r="15" spans="1:18" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>43</v>
@@ -2561,7 +2610,7 @@
     <row r="16" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>51</v>
@@ -2589,7 +2638,7 @@
     <row r="17" spans="1:18" ht="70" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>54</v>
@@ -2639,11 +2688,11 @@
       <c r="B19" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="90"/>
+      <c r="G19" s="89"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -2659,7 +2708,7 @@
     <row r="20" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>40</v>
@@ -2689,7 +2738,7 @@
     <row r="21" spans="1:18" ht="42" x14ac:dyDescent="0.15">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>43</v>
@@ -2727,7 +2776,7 @@
     <row r="22" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="28" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>61</v>
@@ -2755,7 +2804,7 @@
     <row r="23" spans="1:18" ht="70" x14ac:dyDescent="0.15">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>64</v>
@@ -3216,15 +3265,15 @@
   </sheetPr>
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
@@ -3252,7 +3301,7 @@
         <v>70</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>14</v>
@@ -3264,7 +3313,7 @@
         <v>16</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>17</v>
@@ -3294,19 +3343,19 @@
         <v>24</v>
       </c>
       <c r="R1" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="U1" s="8" t="s">
         <v>32</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="W1" s="8" t="s">
         <v>33</v>
@@ -3318,7 +3367,7 @@
         <v>35</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="AA1" s="8" t="s">
         <v>36</v>
@@ -3372,7 +3421,7 @@
       <c r="B3" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>74</v>
       </c>
       <c r="D3" s="20"/>
@@ -3434,7 +3483,7 @@
       <c r="B4" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="91" t="s">
         <v>74</v>
       </c>
       <c r="D4" s="39"/>
@@ -3620,7 +3669,7 @@
       <c r="B8" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="85" t="s">
+      <c r="C8" s="84" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="25"/>
@@ -4122,7 +4171,7 @@
       <c r="B16" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="85" t="s">
+      <c r="C16" s="84" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="25"/>
@@ -4177,12 +4226,12 @@
       </c>
       <c r="AD16" s="25"/>
     </row>
-    <row r="17" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:30" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="69"/>
       <c r="B17" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="84" t="s">
+      <c r="C17" s="83" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="20"/>
@@ -4483,7 +4532,7 @@
       <c r="A23" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="92" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="45" t="s">
@@ -5846,10 +5895,10 @@
       <c r="AD49" s="32"/>
     </row>
     <row r="50" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="94" t="s">
+      <c r="A50" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="95" t="s">
+      <c r="B50" s="94" t="s">
         <v>119</v>
       </c>
       <c r="C50" s="58" t="s">
@@ -5908,7 +5957,7 @@
       <c r="AD50" s="59"/>
     </row>
     <row r="51" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="96" t="s">
+      <c r="A51" s="95" t="s">
         <v>72</v>
       </c>
       <c r="B51" s="65" t="s">
@@ -5968,10 +6017,10 @@
       <c r="AD51" s="62"/>
     </row>
     <row r="52" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="94" t="s">
+      <c r="A52" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="95" t="s">
+      <c r="B52" s="94" t="s">
         <v>121</v>
       </c>
       <c r="C52" s="58" t="s">
@@ -6028,7 +6077,7 @@
       <c r="AD52" s="59"/>
     </row>
     <row r="53" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="96"/>
+      <c r="A53" s="95"/>
       <c r="B53" s="65" t="s">
         <v>122</v>
       </c>
@@ -6084,8 +6133,8 @@
       <c r="AD53" s="66"/>
     </row>
     <row r="54" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="94"/>
-      <c r="B54" s="95" t="s">
+      <c r="A54" s="93"/>
+      <c r="B54" s="94" t="s">
         <v>123</v>
       </c>
       <c r="C54" s="58" t="s">
@@ -6138,7 +6187,7 @@
       <c r="AD54" s="60"/>
     </row>
     <row r="55" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="96"/>
+      <c r="A55" s="95"/>
       <c r="B55" s="65" t="s">
         <v>124</v>
       </c>
@@ -6220,7 +6269,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P37" sqref="P37"/>
+      <selection pane="topRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6245,99 +6294,99 @@
     <col min="23" max="23" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29"/>
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:23" ht="55" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="67"/>
+      <c r="B1" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="75"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="29"/>
+      <c r="B2" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-    </row>
-    <row r="2" spans="1:23" ht="55" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="67"/>
-      <c r="B2" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="75"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="68"/>
@@ -6691,7 +6740,7 @@
       <c r="W11" s="63"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="97"/>
+      <c r="A12" s="96"/>
       <c r="B12" s="22" t="s">
         <v>134</v>
       </c>
@@ -7012,7 +7061,7 @@
       <c r="W20" s="62"/>
     </row>
     <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="97"/>
+      <c r="A21" s="96"/>
       <c r="B21" s="76" t="s">
         <v>135</v>
       </c>
@@ -7136,11 +7185,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7157,130 +7206,125 @@
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
     <col min="13" max="13" width="9.5" customWidth="1"/>
     <col min="14" max="14" width="11.1640625" customWidth="1"/>
-    <col min="15" max="15" width="27.83203125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" customWidth="1"/>
-    <col min="19" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" customWidth="1"/>
-    <col min="22" max="22" width="14.5" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" customWidth="1"/>
-    <col min="24" max="24" width="18.33203125" customWidth="1"/>
-    <col min="25" max="25" width="12.5" customWidth="1"/>
-    <col min="26" max="26" width="14.5" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" customWidth="1"/>
+    <col min="18" max="18" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" customWidth="1"/>
+    <col min="21" max="21" width="14.5" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" customWidth="1"/>
+    <col min="23" max="23" width="18.33203125" customWidth="1"/>
+    <col min="24" max="24" width="12.5" customWidth="1"/>
+    <col min="25" max="25" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="76" t="s">
+    <row r="1" spans="1:25" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="78"/>
+      <c r="B1" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" s="78"/>
+    </row>
+    <row r="2" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="48"/>
+      <c r="B2" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-    </row>
-    <row r="2" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="78"/>
-      <c r="B2" s="75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z2" s="78"/>
-    </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+    </row>
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="42"/>
       <c r="B3" s="79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" s="61" t="s">
         <v>11</v>
@@ -7310,29 +7354,28 @@
         <v>75</v>
       </c>
       <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="O3" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="62"/>
       <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="R3" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="S3" s="62"/>
       <c r="T3" s="62"/>
       <c r="U3" s="62"/>
       <c r="V3" s="62"/>
       <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z3" s="62"/>
-    </row>
-    <row r="4" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+      <c r="X3" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y3" s="62"/>
+    </row>
+    <row r="4" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="44"/>
       <c r="B4" s="80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="58" t="s">
         <v>11</v>
@@ -7362,29 +7405,28 @@
         <v>75</v>
       </c>
       <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="O4" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="59"/>
       <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="R4" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="59"/>
       <c r="T4" s="59"/>
       <c r="U4" s="59"/>
       <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="W4" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="X4" s="59"/>
       <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-    </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="42"/>
       <c r="B5" s="79" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="43" t="s">
         <v>11</v>
@@ -7414,29 +7456,28 @@
         <v>75</v>
       </c>
       <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="O5" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="62"/>
       <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="R5" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="S5" s="62"/>
       <c r="T5" s="62"/>
       <c r="U5" s="62"/>
       <c r="V5" s="62"/>
-      <c r="W5" s="62"/>
-      <c r="X5" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="W5" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="X5" s="62"/>
       <c r="Y5" s="62"/>
-      <c r="Z5" s="62"/>
-    </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="44"/>
       <c r="B6" s="80" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>11</v>
@@ -7462,107 +7503,102 @@
       <c r="L6" s="59"/>
       <c r="M6" s="59"/>
       <c r="N6" s="59"/>
-      <c r="O6" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="O6" s="59"/>
       <c r="P6" s="59"/>
       <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="R6" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="S6" s="59"/>
       <c r="T6" s="59"/>
       <c r="U6" s="59"/>
       <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="W6" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="X6" s="59"/>
       <c r="Y6" s="59"/>
-      <c r="Z6" s="59"/>
-    </row>
-    <row r="7" spans="1:26" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="113"/>
-      <c r="B7" s="114" t="s">
+    </row>
+    <row r="7" spans="1:25" s="107" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="103"/>
+      <c r="B7" s="104" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="106"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="106"/>
+      <c r="Q7" s="106"/>
+      <c r="R7" s="106"/>
+      <c r="S7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="U7" s="106"/>
+      <c r="V7" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="W7" s="106"/>
+      <c r="X7" s="106"/>
+      <c r="Y7" s="106"/>
+    </row>
+    <row r="8" spans="1:25" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="97"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
+      <c r="Y8" s="113"/>
+    </row>
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="99"/>
+      <c r="B9" s="76" t="s">
         <v>151</v>
-      </c>
-      <c r="C7" s="115" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="116"/>
-      <c r="M7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="N7" s="116"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="116"/>
-      <c r="Q7" s="116"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="116"/>
-      <c r="T7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="U7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="V7" s="116"/>
-      <c r="W7" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="X7" s="116"/>
-      <c r="Y7" s="116"/>
-      <c r="Z7" s="116"/>
-    </row>
-    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="98"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="82"/>
-      <c r="R8" s="82"/>
-      <c r="S8" s="82"/>
-      <c r="T8" s="82"/>
-      <c r="U8" s="82"/>
-      <c r="V8" s="82"/>
-      <c r="W8" s="82"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="82"/>
-      <c r="Z8" s="82"/>
-    </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="100"/>
-      <c r="B9" s="76" t="s">
-        <v>152</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="74"/>
@@ -7587,12 +7623,11 @@
       <c r="W9" s="74"/>
       <c r="X9" s="74"/>
       <c r="Y9" s="74"/>
-      <c r="Z9" s="74"/>
-    </row>
-    <row r="10" spans="1:26" s="107" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:25" s="107" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="110"/>
       <c r="B10" s="109" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C10" s="111" t="s">
         <v>11</v>
@@ -7614,37 +7649,36 @@
       <c r="N10" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="O10" s="112"/>
+      <c r="O10" s="112" t="s">
+        <v>75</v>
+      </c>
       <c r="P10" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="Q10" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="T10" s="112"/>
-      <c r="U10" s="112" t="s">
-        <v>75</v>
-      </c>
+      <c r="Q10" s="112"/>
+      <c r="R10" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="S10" s="112"/>
+      <c r="T10" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="U10" s="112"/>
       <c r="V10" s="112"/>
-      <c r="W10" s="112"/>
+      <c r="W10" s="112" t="s">
+        <v>75</v>
+      </c>
       <c r="X10" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="Y10" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z10" s="112"/>
-    </row>
-    <row r="11" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y10" s="112"/>
+    </row>
+    <row r="11" spans="1:25" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="44"/>
       <c r="B11" s="80" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="83" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="82" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="59"/>
@@ -7664,26 +7698,25 @@
       <c r="N11" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="59"/>
+      <c r="O11" s="59" t="s">
+        <v>75</v>
+      </c>
       <c r="P11" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="Q11" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="Q11" s="59"/>
       <c r="R11" s="59"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="S11" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" s="59"/>
       <c r="U11" s="59"/>
-      <c r="V11" s="59"/>
-      <c r="W11" s="59" t="s">
-        <v>75</v>
-      </c>
+      <c r="V11" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" s="59"/>
       <c r="X11" s="59"/>
       <c r="Y11" s="59"/>
-      <c r="Z11" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -7698,11 +7731,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U12" sqref="U12"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7733,123 +7766,123 @@
     <col min="27" max="27" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="29"/>
-      <c r="B1" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-    </row>
-    <row r="2" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="101"/>
-      <c r="B2" s="75" t="s">
+    <row r="1" spans="1:27" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="100"/>
+      <c r="B1" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="I1" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="T2" s="8" t="s">
+      <c r="S1" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="W2" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="X2" s="8" t="s">
+      <c r="W1" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="X1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="102"/>
+      <c r="AA1" s="101"/>
+    </row>
+    <row r="2" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="29"/>
+      <c r="B2" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
     </row>
     <row r="3" spans="1:27" s="107" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A3" s="104"/>
-      <c r="B3" s="105" t="s">
-        <v>156</v>
+      <c r="A3" s="103"/>
+      <c r="B3" s="104" t="s">
+        <v>168</v>
       </c>
       <c r="C3" s="108" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D3" s="106"/>
       <c r="E3" s="106" t="s">
@@ -7891,10 +7924,10 @@
     <row r="4" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="44"/>
       <c r="B4" s="80" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" s="92" t="s">
-        <v>157</v>
+        <v>170</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>169</v>
       </c>
       <c r="D4" s="59"/>
       <c r="E4" s="59" t="s">
@@ -7946,10 +7979,10 @@
     <row r="5" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="42"/>
       <c r="B5" s="79" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="103" t="s">
-        <v>157</v>
+        <v>171</v>
+      </c>
+      <c r="C5" s="102" t="s">
+        <v>169</v>
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62" t="s">
@@ -8003,10 +8036,10 @@
     <row r="6" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="44"/>
       <c r="B6" s="80" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" s="92" t="s">
-        <v>157</v>
+        <v>172</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>169</v>
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="59" t="s">
@@ -8058,10 +8091,10 @@
     <row r="7" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="40"/>
       <c r="B7" s="79" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D7" s="73"/>
       <c r="E7" s="73" t="s">
@@ -8113,10 +8146,10 @@
     <row r="8" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="53"/>
       <c r="B8" s="80" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="39" t="s">
@@ -8164,10 +8197,10 @@
     <row r="9" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="40"/>
       <c r="B9" s="79" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D9" s="73"/>
       <c r="E9" s="73" t="s">
@@ -8213,38 +8246,38 @@
       <c r="AA9" s="63"/>
     </row>
     <row r="10" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="98"/>
+      <c r="A10" s="97"/>
       <c r="B10" s="80"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="82"/>
-      <c r="T10" s="82"/>
-      <c r="U10" s="82"/>
-      <c r="V10" s="82"/>
-      <c r="W10" s="82"/>
-      <c r="X10" s="82"/>
-      <c r="Y10" s="82"/>
-      <c r="Z10" s="82"/>
-      <c r="AA10" s="82"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="81"/>
+      <c r="AA10" s="81"/>
     </row>
     <row r="11" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="100"/>
+      <c r="A11" s="99"/>
       <c r="B11" s="76" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="74"/>
@@ -8272,328 +8305,397 @@
       <c r="Z11" s="74"/>
       <c r="AA11" s="74"/>
     </row>
-    <row r="12" spans="1:27" s="107" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="104"/>
-      <c r="B12" s="105" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="108" t="s">
+    <row r="12" spans="1:27" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="R12" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA12" s="106"/>
-    </row>
-    <row r="13" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="44"/>
-      <c r="B13" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="92" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA13" s="59"/>
+      <c r="M12" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z12" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA12" s="8"/>
+    </row>
+    <row r="13" spans="1:27" s="107" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="103"/>
+      <c r="B13" s="104" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="108" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="R13" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="S13" s="106"/>
+      <c r="T13" s="106"/>
+      <c r="U13" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="V13" s="106"/>
+      <c r="W13" s="106"/>
+      <c r="X13" s="106"/>
+      <c r="Y13" s="106"/>
+      <c r="Z13" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA13" s="106"/>
     </row>
     <row r="14" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="69"/>
-      <c r="B14" s="79" t="s">
-        <v>167</v>
-      </c>
-      <c r="C14" s="103" t="s">
-        <v>157</v>
-      </c>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="62"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="R14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="S14" s="62"/>
-      <c r="T14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="U14" s="62"/>
-      <c r="V14" s="62"/>
-      <c r="W14" s="62"/>
-      <c r="X14" s="62"/>
-      <c r="Y14" s="62"/>
-      <c r="Z14" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA14" s="62"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="80" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="59"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA14" s="59"/>
     </row>
     <row r="15" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="71"/>
-      <c r="B15" s="80" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="92" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="U15" s="59"/>
-      <c r="V15" s="59"/>
-      <c r="W15" s="59"/>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA15" s="59"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="79" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="102" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="R15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="U15" s="62"/>
+      <c r="V15" s="62"/>
+      <c r="W15" s="62"/>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA15" s="62"/>
     </row>
     <row r="16" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="69"/>
-      <c r="B16" s="79" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="91" t="s">
         <v>169</v>
       </c>
-      <c r="C16" s="103" t="s">
-        <v>157</v>
-      </c>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="R16" s="62"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="U16" s="62"/>
-      <c r="V16" s="62"/>
-      <c r="W16" s="62"/>
-      <c r="X16" s="62"/>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA16" s="62"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="U16" s="59"/>
+      <c r="V16" s="59"/>
+      <c r="W16" s="59"/>
+      <c r="X16" s="59"/>
+      <c r="Y16" s="59"/>
+      <c r="Z16" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA16" s="59"/>
     </row>
     <row r="17" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="71"/>
-      <c r="B17" s="80" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="92" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="R17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="S17" s="59"/>
-      <c r="T17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="U17" s="59"/>
-      <c r="V17" s="59"/>
-      <c r="W17" s="59"/>
-      <c r="X17" s="59"/>
-      <c r="Y17" s="59"/>
-      <c r="Z17" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA17" s="59"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="102" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
+      <c r="W17" s="62"/>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA17" s="62"/>
     </row>
     <row r="18" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="69"/>
-      <c r="B18" s="79" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="103" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="62"/>
-      <c r="O18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="R18" s="62"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="V18" s="62"/>
-      <c r="W18" s="62"/>
-      <c r="X18" s="62"/>
-      <c r="Y18" s="62"/>
-      <c r="Z18" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA18" s="62"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="80" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="91" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="R18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="U18" s="59"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" s="59"/>
+    </row>
+    <row r="19" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="69"/>
+      <c r="B19" s="79" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" s="102" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="V19" s="62"/>
+      <c r="W19" s="62"/>
+      <c r="X19" s="62"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA19" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -8604,28 +8706,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2c089627-9960-44e1-9762-bfa3ba590a63">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D558A0C25AD9694BB62FFB42927C2A24" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd42f41f2bb46cd63a6e8ca5b25a11d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c089627-9960-44e1-9762-bfa3ba590a63" xmlns:ns3="64211953-cb0a-4a02-b1d5-47de0f0a68d5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd994a08d1fe56e517ba8eea0123f9e" ns2:_="" ns3:_="">
     <xsd:import namespace="2c089627-9960-44e1-9762-bfa3ba590a63"/>
@@ -8872,26 +8952,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D20332E-DAE9-4FA3-898D-66D0C67FC073}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="64211953-cb0a-4a02-b1d5-47de0f0a68d5"/>
-    <ds:schemaRef ds:uri="2c089627-9960-44e1-9762-bfa3ba590a63"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E72343A-1D3E-4810-AF97-187893FA4160}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2c089627-9960-44e1-9762-bfa3ba590a63">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C868719-05F4-42CE-A730-B62E340093D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8908,4 +8991,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E72343A-1D3E-4810-AF97-187893FA4160}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D20332E-DAE9-4FA3-898D-66D0C67FC073}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="64211953-cb0a-4a02-b1d5-47de0f0a68d5"/>
+    <ds:schemaRef ds:uri="2c089627-9960-44e1-9762-bfa3ba590a63"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cập nhật tệp Excel, cải thiện quy trình kiểm tra trong test_help_me_choose.py, bổ sung các loại xe mới vào model.example.json và điều chỉnh các tham số trong conftest.py để tối ưu hóa hiệu suất.
</commit_message>
<xml_diff>
--- a/Bike Chooser _ Honda Powersports - Street.xlsx
+++ b/Bike Chooser _ Honda Powersports - Street.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gg\honda-help-me-choose-automate-testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dat.ta/Desktop/code/work/honda-help-me-choose-automate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1E93A4-FD9E-4CEE-9305-A3D7C29CB3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7336EC7-27EF-A84B-A9AA-9CFD1586E700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46020" yWindow="2960" windowWidth="23260" windowHeight="12460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUESTIONS" sheetId="1" r:id="rId1"/>
@@ -4175,9 +4175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4215,7 +4215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4321,7 +4321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4463,7 +4463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4481,24 +4481,24 @@
       <selection pane="topRight" activeCell="C15" sqref="C15:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="27.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="18" width="14.44140625" customWidth="1"/>
+    <col min="15" max="18" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -4518,7 +4518,7 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -4556,7 +4556,7 @@
       <c r="Q2" s="7"/>
       <c r="R2" s="9"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>9</v>
@@ -4584,7 +4584,7 @@
       <c r="Q3" s="20"/>
       <c r="R3" s="20"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="84"/>
@@ -4604,7 +4604,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="22"/>
       <c r="B5" s="76" t="s">
         <v>13</v>
@@ -4626,7 +4626,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>171</v>
@@ -4654,7 +4654,7 @@
       <c r="Q6" s="20"/>
       <c r="R6" s="20"/>
     </row>
-    <row r="7" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>172</v>
@@ -4692,7 +4692,7 @@
       <c r="Q7" s="49"/>
       <c r="R7" s="49"/>
     </row>
-    <row r="8" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>183</v>
@@ -4724,7 +4724,7 @@
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="16"/>
       <c r="B9" s="17" t="s">
         <v>184</v>
@@ -4752,7 +4752,7 @@
       <c r="Q9" s="49"/>
       <c r="R9" s="49"/>
     </row>
-    <row r="10" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="18"/>
       <c r="B10" s="11" t="s">
         <v>173</v>
@@ -4780,7 +4780,7 @@
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
     </row>
-    <row r="11" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
         <v>174</v>
@@ -4808,7 +4808,7 @@
       <c r="Q11" s="49"/>
       <c r="R11" s="49"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="77"/>
       <c r="C12" s="20"/>
@@ -4828,7 +4828,7 @@
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
         <v>39</v>
@@ -4850,7 +4850,7 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>175</v>
@@ -4878,7 +4878,7 @@
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
     </row>
-    <row r="15" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>176</v>
@@ -4916,7 +4916,7 @@
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="12"/>
       <c r="B16" s="13" t="s">
         <v>177</v>
@@ -4944,7 +4944,7 @@
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
     </row>
-    <row r="17" spans="1:18" ht="66" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="70" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>178</v>
@@ -4972,7 +4972,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="27"/>
@@ -4992,7 +4992,7 @@
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="22"/>
       <c r="B19" s="76" t="s">
         <v>57</v>
@@ -5014,7 +5014,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
         <v>179</v>
@@ -5044,7 +5044,7 @@
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
     </row>
-    <row r="21" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="42" x14ac:dyDescent="0.15">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
         <v>180</v>
@@ -5082,7 +5082,7 @@
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
     </row>
-    <row r="22" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="28" t="s">
         <v>181</v>
@@ -5110,7 +5110,7 @@
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
     </row>
-    <row r="23" spans="1:18" ht="66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="70" x14ac:dyDescent="0.15">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>182</v>
@@ -5138,7 +5138,7 @@
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -5158,7 +5158,7 @@
       <c r="Q24" s="29"/>
       <c r="R24" s="29"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -5178,7 +5178,7 @@
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
@@ -5198,7 +5198,7 @@
       <c r="Q26" s="29"/>
       <c r="R26" s="29"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
@@ -5218,7 +5218,7 @@
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -5238,7 +5238,7 @@
       <c r="Q28" s="29"/>
       <c r="R28" s="29"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" s="29"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -5258,7 +5258,7 @@
       <c r="Q29" s="29"/>
       <c r="R29" s="29"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" s="29"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -5278,7 +5278,7 @@
       <c r="Q30" s="29"/>
       <c r="R30" s="29"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -5298,7 +5298,7 @@
       <c r="Q31" s="29"/>
       <c r="R31" s="29"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -5318,7 +5318,7 @@
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -5338,7 +5338,7 @@
       <c r="Q33" s="29"/>
       <c r="R33" s="29"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
@@ -5358,7 +5358,7 @@
       <c r="Q34" s="29"/>
       <c r="R34" s="29"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35" s="29"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
@@ -5378,7 +5378,7 @@
       <c r="Q35" s="29"/>
       <c r="R35" s="29"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36" s="29"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
@@ -5398,7 +5398,7 @@
       <c r="Q36" s="29"/>
       <c r="R36" s="29"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -5418,7 +5418,7 @@
       <c r="Q37" s="29"/>
       <c r="R37" s="29"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
@@ -5438,7 +5438,7 @@
       <c r="Q38" s="29"/>
       <c r="R38" s="29"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39" s="29"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
@@ -5458,7 +5458,7 @@
       <c r="Q39" s="29"/>
       <c r="R39" s="29"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -5478,7 +5478,7 @@
       <c r="Q40" s="29"/>
       <c r="R40" s="29"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
@@ -5498,7 +5498,7 @@
       <c r="Q41" s="29"/>
       <c r="R41" s="29"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42" s="29"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -5518,7 +5518,7 @@
       <c r="Q42" s="29"/>
       <c r="R42" s="29"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -5538,7 +5538,7 @@
       <c r="Q43" s="29"/>
       <c r="R43" s="29"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
@@ -5579,27 +5579,27 @@
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
+    <col min="8" max="9" width="13.5" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
-    <col min="16" max="22" width="14.44140625" customWidth="1"/>
+    <col min="16" max="22" width="14.5" customWidth="1"/>
     <col min="23" max="24" width="11.6640625" customWidth="1"/>
-    <col min="25" max="30" width="14.44140625" customWidth="1"/>
+    <col min="25" max="30" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
         <v>68</v>
       </c>
@@ -5687,7 +5687,7 @@
       <c r="AC1" s="8"/>
       <c r="AD1" s="8"/>
     </row>
-    <row r="2" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31" t="s">
         <v>67</v>
@@ -5721,7 +5721,7 @@
       <c r="AC2" s="32"/>
       <c r="AD2" s="32"/>
     </row>
-    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>71</v>
       </c>
@@ -5781,7 +5781,7 @@
       <c r="AC3" s="20"/>
       <c r="AD3" s="20"/>
     </row>
-    <row r="4" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="37" t="s">
         <v>71</v>
       </c>
@@ -5841,7 +5841,7 @@
       <c r="AC4" s="59"/>
       <c r="AD4" s="59"/>
     </row>
-    <row r="5" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="40"/>
       <c r="B5" s="41"/>
       <c r="C5" s="42"/>
@@ -5873,7 +5873,7 @@
       <c r="AC5" s="42"/>
       <c r="AD5" s="42"/>
     </row>
-    <row r="6" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="31"/>
       <c r="B6" s="23" t="s">
         <v>76</v>
@@ -5907,7 +5907,7 @@
       <c r="AC6" s="32"/>
       <c r="AD6" s="32"/>
     </row>
-    <row r="7" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="69" t="s">
         <v>71</v>
       </c>
@@ -5969,7 +5969,7 @@
       <c r="AC7" s="20"/>
       <c r="AD7" s="20"/>
     </row>
-    <row r="8" spans="1:30" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="71"/>
       <c r="B8" s="19" t="s">
         <v>78</v>
@@ -6029,7 +6029,7 @@
       <c r="AC8" s="25"/>
       <c r="AD8" s="25"/>
     </row>
-    <row r="9" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="69" t="s">
         <v>71</v>
       </c>
@@ -6095,7 +6095,7 @@
       <c r="AC9" s="20"/>
       <c r="AD9" s="20"/>
     </row>
-    <row r="10" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="71" t="s">
         <v>71</v>
       </c>
@@ -6161,7 +6161,7 @@
       <c r="AC10" s="25"/>
       <c r="AD10" s="25"/>
     </row>
-    <row r="11" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="69" t="s">
         <v>71</v>
       </c>
@@ -6225,7 +6225,7 @@
       <c r="AC11" s="20"/>
       <c r="AD11" s="20"/>
     </row>
-    <row r="12" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="71" t="s">
         <v>71</v>
       </c>
@@ -6287,7 +6287,7 @@
       <c r="AC12" s="25"/>
       <c r="AD12" s="25"/>
     </row>
-    <row r="13" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="69" t="s">
         <v>71</v>
       </c>
@@ -6349,7 +6349,7 @@
       <c r="AC13" s="20"/>
       <c r="AD13" s="20"/>
     </row>
-    <row r="14" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="71" t="s">
         <v>71</v>
       </c>
@@ -6411,7 +6411,7 @@
       <c r="AC14" s="25"/>
       <c r="AD14" s="25"/>
     </row>
-    <row r="15" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="69"/>
       <c r="B15" s="51" t="s">
         <v>85</v>
@@ -6471,7 +6471,7 @@
       <c r="AC15" s="20"/>
       <c r="AD15" s="20"/>
     </row>
-    <row r="16" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="71"/>
       <c r="B16" s="50" t="s">
         <v>86</v>
@@ -6531,7 +6531,7 @@
       <c r="AC16" s="25"/>
       <c r="AD16" s="25"/>
     </row>
-    <row r="17" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="69"/>
       <c r="B17" s="51" t="s">
         <v>87</v>
@@ -6589,7 +6589,7 @@
       <c r="AC17" s="20"/>
       <c r="AD17" s="20"/>
     </row>
-    <row r="18" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="46"/>
       <c r="B18" s="47"/>
       <c r="C18" s="48"/>
@@ -6621,7 +6621,7 @@
       <c r="AC18" s="48"/>
       <c r="AD18" s="48"/>
     </row>
-    <row r="19" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="31"/>
       <c r="B19" s="31" t="s">
         <v>88</v>
@@ -6655,7 +6655,7 @@
       <c r="AC19" s="32"/>
       <c r="AD19" s="32"/>
     </row>
-    <row r="20" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="69" t="s">
         <v>71</v>
       </c>
@@ -6711,7 +6711,7 @@
       <c r="AC20" s="20"/>
       <c r="AD20" s="20"/>
     </row>
-    <row r="21" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="71" t="s">
         <v>71</v>
       </c>
@@ -6769,7 +6769,7 @@
       <c r="AC21" s="25"/>
       <c r="AD21" s="25"/>
     </row>
-    <row r="22" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="69" t="s">
         <v>71</v>
       </c>
@@ -6827,7 +6827,7 @@
       <c r="AC22" s="20"/>
       <c r="AD22" s="20"/>
     </row>
-    <row r="23" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>71</v>
       </c>
@@ -6889,7 +6889,7 @@
       <c r="AC23" s="25"/>
       <c r="AD23" s="25"/>
     </row>
-    <row r="24" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="69"/>
       <c r="B24" s="51" t="s">
         <v>93</v>
@@ -6945,7 +6945,7 @@
       <c r="AC24" s="20"/>
       <c r="AD24" s="20"/>
     </row>
-    <row r="25" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="71"/>
       <c r="B25" s="50" t="s">
         <v>94</v>
@@ -7001,7 +7001,7 @@
       <c r="AC25" s="25"/>
       <c r="AD25" s="25"/>
     </row>
-    <row r="26" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="69"/>
       <c r="B26" s="51" t="s">
         <v>95</v>
@@ -7055,7 +7055,7 @@
       <c r="AC26" s="20"/>
       <c r="AD26" s="20"/>
     </row>
-    <row r="27" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="71"/>
       <c r="B27" s="50"/>
       <c r="C27" s="25"/>
@@ -7087,7 +7087,7 @@
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
     </row>
-    <row r="28" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="22"/>
       <c r="B28" s="31" t="s">
         <v>96</v>
@@ -7121,7 +7121,7 @@
       <c r="AC28" s="32"/>
       <c r="AD28" s="32"/>
     </row>
-    <row r="29" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="71" t="s">
         <v>97</v>
       </c>
@@ -7179,7 +7179,7 @@
       <c r="AC29" s="25"/>
       <c r="AD29" s="25"/>
     </row>
-    <row r="30" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="69" t="s">
         <v>99</v>
       </c>
@@ -7237,7 +7237,7 @@
       <c r="AC30" s="20"/>
       <c r="AD30" s="20"/>
     </row>
-    <row r="31" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="71"/>
       <c r="B31" s="50" t="s">
         <v>101</v>
@@ -7289,7 +7289,7 @@
       <c r="AC31" s="25"/>
       <c r="AD31" s="25"/>
     </row>
-    <row r="32" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="40"/>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -7321,7 +7321,7 @@
       <c r="AC32" s="42"/>
       <c r="AD32" s="42"/>
     </row>
-    <row r="33" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="31"/>
       <c r="B33" s="31" t="s">
         <v>102</v>
@@ -7355,7 +7355,7 @@
       <c r="AC33" s="32"/>
       <c r="AD33" s="32"/>
     </row>
-    <row r="34" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="71" t="s">
         <v>71</v>
       </c>
@@ -7415,7 +7415,7 @@
       <c r="AC34" s="25"/>
       <c r="AD34" s="25"/>
     </row>
-    <row r="35" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="69" t="s">
         <v>71</v>
       </c>
@@ -7475,7 +7475,7 @@
       <c r="AC35" s="20"/>
       <c r="AD35" s="20"/>
     </row>
-    <row r="36" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="71" t="s">
         <v>71</v>
       </c>
@@ -7535,7 +7535,7 @@
       <c r="AC36" s="25"/>
       <c r="AD36" s="25"/>
     </row>
-    <row r="37" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="69" t="s">
         <v>71</v>
       </c>
@@ -7591,7 +7591,7 @@
       <c r="AC37" s="20"/>
       <c r="AD37" s="20"/>
     </row>
-    <row r="38" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="71"/>
       <c r="B38" s="50" t="s">
         <v>107</v>
@@ -7649,7 +7649,7 @@
       <c r="AC38" s="25"/>
       <c r="AD38" s="25"/>
     </row>
-    <row r="39" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="69" t="s">
         <v>71</v>
       </c>
@@ -7709,7 +7709,7 @@
       <c r="AC39" s="20"/>
       <c r="AD39" s="20"/>
     </row>
-    <row r="40" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="71" t="s">
         <v>71</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="AC40" s="25"/>
       <c r="AD40" s="25"/>
     </row>
-    <row r="41" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="69" t="s">
         <v>71</v>
       </c>
@@ -7825,7 +7825,7 @@
       <c r="AC41" s="20"/>
       <c r="AD41" s="20"/>
     </row>
-    <row r="42" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="53"/>
       <c r="B42" s="54"/>
       <c r="C42" s="44"/>
@@ -7857,7 +7857,7 @@
       <c r="AC42" s="25"/>
       <c r="AD42" s="25"/>
     </row>
-    <row r="43" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="31"/>
       <c r="B43" s="31" t="s">
         <v>111</v>
@@ -7891,7 +7891,7 @@
       <c r="AC43" s="32"/>
       <c r="AD43" s="32"/>
     </row>
-    <row r="44" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="69" t="s">
         <v>71</v>
       </c>
@@ -7951,7 +7951,7 @@
       <c r="AC44" s="20"/>
       <c r="AD44" s="20"/>
     </row>
-    <row r="45" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="71" t="s">
         <v>71</v>
       </c>
@@ -8005,7 +8005,7 @@
       <c r="AC45" s="25"/>
       <c r="AD45" s="25"/>
     </row>
-    <row r="46" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="69" t="s">
         <v>71</v>
       </c>
@@ -8059,7 +8059,7 @@
       <c r="AC46" s="55"/>
       <c r="AD46" s="55"/>
     </row>
-    <row r="47" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="71"/>
       <c r="B47" s="50" t="s">
         <v>115</v>
@@ -8117,7 +8117,7 @@
       <c r="AC47" s="56"/>
       <c r="AD47" s="56"/>
     </row>
-    <row r="48" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="42"/>
       <c r="B48" s="57"/>
       <c r="C48" s="42"/>
@@ -8149,7 +8149,7 @@
       <c r="AC48" s="42"/>
       <c r="AD48" s="42"/>
     </row>
-    <row r="49" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="31"/>
       <c r="B49" s="31" t="s">
         <v>116</v>
@@ -8183,7 +8183,7 @@
       <c r="AC49" s="32"/>
       <c r="AD49" s="32"/>
     </row>
-    <row r="50" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="93" t="s">
         <v>71</v>
       </c>
@@ -8243,7 +8243,7 @@
       <c r="AC50" s="59"/>
       <c r="AD50" s="59"/>
     </row>
-    <row r="51" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="95" t="s">
         <v>71</v>
       </c>
@@ -8301,7 +8301,7 @@
       <c r="AC51" s="62"/>
       <c r="AD51" s="62"/>
     </row>
-    <row r="52" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="93" t="s">
         <v>71</v>
       </c>
@@ -8359,7 +8359,7 @@
       <c r="AC52" s="59"/>
       <c r="AD52" s="59"/>
     </row>
-    <row r="53" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="95"/>
       <c r="B53" s="65" t="s">
         <v>120</v>
@@ -8415,7 +8415,7 @@
       <c r="AC53" s="66"/>
       <c r="AD53" s="66"/>
     </row>
-    <row r="54" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="93"/>
       <c r="B54" s="94" t="s">
         <v>121</v>
@@ -8469,7 +8469,7 @@
       <c r="AC54" s="60"/>
       <c r="AD54" s="60"/>
     </row>
-    <row r="55" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="95"/>
       <c r="B55" s="65" t="s">
         <v>122</v>
@@ -8555,28 +8555,28 @@
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
     <col min="14" max="15" width="17.33203125" customWidth="1"/>
-    <col min="16" max="18" width="14.44140625" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="16" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
     <col min="20" max="20" width="10.6640625" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="14.44140625" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="55" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="67"/>
       <c r="B1" s="75" t="s">
         <v>69</v>
@@ -8640,7 +8640,7 @@
       </c>
       <c r="V1" s="75"/>
     </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29"/>
       <c r="B2" s="22" t="s">
         <v>123</v>
@@ -8666,7 +8666,7 @@
       <c r="U2" s="32"/>
       <c r="V2" s="32"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="68"/>
       <c r="B3" s="69" t="s">
         <v>124</v>
@@ -8708,7 +8708,7 @@
       </c>
       <c r="V3" s="62"/>
     </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70"/>
       <c r="B4" s="71" t="s">
         <v>125</v>
@@ -8748,7 +8748,7 @@
       </c>
       <c r="V4" s="59"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="68"/>
       <c r="B5" s="69" t="s">
         <v>126</v>
@@ -8788,7 +8788,7 @@
       <c r="U5" s="62"/>
       <c r="V5" s="62"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70"/>
       <c r="B6" s="71" t="s">
         <v>127</v>
@@ -8828,7 +8828,7 @@
       </c>
       <c r="V6" s="59"/>
     </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="68"/>
       <c r="B7" s="69" t="s">
         <v>128</v>
@@ -8868,7 +8868,7 @@
       <c r="U7" s="62"/>
       <c r="V7" s="62"/>
     </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="70"/>
       <c r="B8" s="71" t="s">
         <v>129</v>
@@ -8908,7 +8908,7 @@
       <c r="U8" s="59"/>
       <c r="V8" s="59"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="68"/>
       <c r="B9" s="69" t="s">
         <v>130</v>
@@ -8944,7 +8944,7 @@
       <c r="U9" s="62"/>
       <c r="V9" s="62"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="70"/>
       <c r="B10" s="71" t="s">
         <v>131</v>
@@ -8980,7 +8980,7 @@
       <c r="U10" s="59"/>
       <c r="V10" s="59"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="72"/>
       <c r="B11" s="69"/>
       <c r="C11" s="73"/>
@@ -9004,7 +9004,7 @@
       <c r="U11" s="63"/>
       <c r="V11" s="63"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="96"/>
       <c r="B12" s="22" t="s">
         <v>132</v>
@@ -9030,7 +9030,7 @@
       <c r="U12" s="74"/>
       <c r="V12" s="74"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="70"/>
       <c r="B13" s="71" t="s">
         <v>134</v>
@@ -9068,7 +9068,7 @@
       </c>
       <c r="V13" s="59"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="68"/>
       <c r="B14" s="69" t="s">
         <v>135</v>
@@ -9106,7 +9106,7 @@
       </c>
       <c r="V14" s="62"/>
     </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="70"/>
       <c r="B15" s="71" t="s">
         <v>136</v>
@@ -9144,7 +9144,7 @@
       </c>
       <c r="V15" s="59"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="68"/>
       <c r="B16" s="69" t="s">
         <v>137</v>
@@ -9182,7 +9182,7 @@
       </c>
       <c r="V16" s="62"/>
     </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="70"/>
       <c r="B17" s="71" t="s">
         <v>138</v>
@@ -9220,7 +9220,7 @@
       </c>
       <c r="V17" s="59"/>
     </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="68"/>
       <c r="B18" s="69" t="s">
         <v>139</v>
@@ -9256,7 +9256,7 @@
       <c r="U18" s="62"/>
       <c r="V18" s="62"/>
     </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="70"/>
       <c r="B19" s="71" t="s">
         <v>140</v>
@@ -9292,7 +9292,7 @@
       <c r="U19" s="59"/>
       <c r="V19" s="59"/>
     </row>
-    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="68"/>
       <c r="B20" s="79"/>
       <c r="C20" s="73"/>
@@ -9316,7 +9316,7 @@
       <c r="U20" s="62"/>
       <c r="V20" s="62"/>
     </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="96"/>
       <c r="B21" s="76" t="s">
         <v>133</v>
@@ -9342,7 +9342,7 @@
       <c r="U21" s="74"/>
       <c r="V21" s="74"/>
     </row>
-    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70"/>
       <c r="B22" s="80" t="s">
         <v>141</v>
@@ -9382,7 +9382,7 @@
       </c>
       <c r="V22" s="59"/>
     </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="68"/>
       <c r="B23" s="77" t="s">
         <v>142</v>
@@ -9445,34 +9445,34 @@
       <selection pane="topRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="9" width="13.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
     <col min="16" max="16" width="8.33203125" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" customWidth="1"/>
+    <col min="18" max="18" width="10.5" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" customWidth="1"/>
-    <col min="20" max="20" width="9.77734375" customWidth="1"/>
-    <col min="21" max="21" width="14.44140625" customWidth="1"/>
-    <col min="22" max="22" width="15.77734375" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" customWidth="1"/>
+    <col min="21" max="21" width="14.5" customWidth="1"/>
+    <col min="22" max="22" width="15.83203125" customWidth="1"/>
     <col min="23" max="23" width="18.33203125" customWidth="1"/>
-    <col min="24" max="24" width="12.44140625" customWidth="1"/>
-    <col min="25" max="25" width="14.44140625" customWidth="1"/>
+    <col min="24" max="24" width="12.5" customWidth="1"/>
+    <col min="25" max="25" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="78"/>
       <c r="B1" s="75" t="s">
         <v>69</v>
@@ -9545,7 +9545,7 @@
       </c>
       <c r="Y1" s="78"/>
     </row>
-    <row r="2" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="76" t="s">
         <v>143</v>
@@ -9574,7 +9574,7 @@
       <c r="X2" s="32"/>
       <c r="Y2" s="32"/>
     </row>
-    <row r="3" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="42"/>
       <c r="B3" s="79" t="s">
         <v>144</v>
@@ -9625,7 +9625,7 @@
       </c>
       <c r="Y3" s="62"/>
     </row>
-    <row r="4" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="44"/>
       <c r="B4" s="80" t="s">
         <v>145</v>
@@ -9676,7 +9676,7 @@
       <c r="X4" s="59"/>
       <c r="Y4" s="59"/>
     </row>
-    <row r="5" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="42"/>
       <c r="B5" s="79" t="s">
         <v>146</v>
@@ -9727,7 +9727,7 @@
       <c r="X5" s="62"/>
       <c r="Y5" s="62"/>
     </row>
-    <row r="6" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="44"/>
       <c r="B6" s="80" t="s">
         <v>147</v>
@@ -9772,7 +9772,7 @@
       <c r="X6" s="59"/>
       <c r="Y6" s="59"/>
     </row>
-    <row r="7" spans="1:25" s="106" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" s="106" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="102"/>
       <c r="B7" s="103" t="s">
         <v>148</v>
@@ -9821,7 +9821,7 @@
       <c r="X7" s="105"/>
       <c r="Y7" s="105"/>
     </row>
-    <row r="8" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="97"/>
       <c r="B8" s="112"/>
       <c r="C8" s="112"/>
@@ -9848,7 +9848,7 @@
       <c r="X8" s="112"/>
       <c r="Y8" s="112"/>
     </row>
-    <row r="9" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="99"/>
       <c r="B9" s="76" t="s">
         <v>149</v>
@@ -9877,7 +9877,7 @@
       <c r="X9" s="74"/>
       <c r="Y9" s="74"/>
     </row>
-    <row r="10" spans="1:25" s="106" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="106" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="109"/>
       <c r="B10" s="108" t="s">
         <v>150</v>
@@ -9926,7 +9926,7 @@
       </c>
       <c r="Y10" s="111"/>
     </row>
-    <row r="11" spans="1:25" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="44"/>
       <c r="B11" s="80" t="s">
         <v>151</v>
@@ -9988,36 +9988,36 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C20" sqref="C20"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
+    <col min="8" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" customWidth="1"/>
-    <col min="17" max="17" width="8.77734375" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="8.83203125" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" customWidth="1"/>
     <col min="19" max="19" width="13.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.109375" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" customWidth="1"/>
     <col min="21" max="21" width="13.6640625" customWidth="1"/>
-    <col min="22" max="22" width="14.44140625" customWidth="1"/>
-    <col min="23" max="23" width="17.44140625" customWidth="1"/>
-    <col min="24" max="24" width="18.44140625" customWidth="1"/>
-    <col min="25" max="26" width="17.77734375" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="23" max="23" width="17.5" customWidth="1"/>
+    <col min="24" max="24" width="18.5" customWidth="1"/>
+    <col min="25" max="26" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="100"/>
       <c r="B1" s="75" t="s">
         <v>69</v>
@@ -10093,7 +10093,7 @@
       </c>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="29"/>
       <c r="B2" s="76" t="s">
         <v>152</v>
@@ -10123,7 +10123,7 @@
       <c r="Y2" s="32"/>
       <c r="Z2" s="32"/>
     </row>
-    <row r="3" spans="1:26" s="106" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="106" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="102"/>
       <c r="B3" s="103" t="s">
         <v>153</v>
@@ -10167,7 +10167,7 @@
       </c>
       <c r="Z3" s="105"/>
     </row>
-    <row r="4" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="44"/>
       <c r="B4" s="80" t="s">
         <v>155</v>
@@ -10221,7 +10221,7 @@
       </c>
       <c r="Z4" s="59"/>
     </row>
-    <row r="5" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="42"/>
       <c r="B5" s="79" t="s">
         <v>156</v>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="Z5" s="62"/>
     </row>
-    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="44"/>
       <c r="B6" s="80" t="s">
         <v>157</v>
@@ -10331,7 +10331,7 @@
       <c r="Y6" s="59"/>
       <c r="Z6" s="59"/>
     </row>
-    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="40"/>
       <c r="B7" s="79" t="s">
         <v>158</v>
@@ -10385,7 +10385,7 @@
       <c r="Y7" s="63"/>
       <c r="Z7" s="63"/>
     </row>
-    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="53"/>
       <c r="B8" s="80" t="s">
         <v>159</v>
@@ -10435,7 +10435,7 @@
       <c r="Y8" s="64"/>
       <c r="Z8" s="64"/>
     </row>
-    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="40"/>
       <c r="B9" s="79" t="s">
         <v>160</v>
@@ -10485,7 +10485,7 @@
       <c r="Y9" s="63"/>
       <c r="Z9" s="63"/>
     </row>
-    <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="97"/>
       <c r="B10" s="80"/>
       <c r="C10" s="98"/>
@@ -10513,7 +10513,7 @@
       <c r="Y10" s="81"/>
       <c r="Z10" s="81"/>
     </row>
-    <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="99"/>
       <c r="B11" s="76" t="s">
         <v>161</v>
@@ -10543,7 +10543,7 @@
       <c r="Y11" s="74"/>
       <c r="Z11" s="74"/>
     </row>
-    <row r="12" spans="1:26" s="106" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="106" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="102"/>
       <c r="B12" s="103" t="s">
         <v>162</v>
@@ -10587,7 +10587,7 @@
       </c>
       <c r="Z12" s="105"/>
     </row>
-    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="44"/>
       <c r="B13" s="80" t="s">
         <v>163</v>
@@ -10631,7 +10631,7 @@
       </c>
       <c r="Z13" s="59"/>
     </row>
-    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="69"/>
       <c r="B14" s="79" t="s">
         <v>164</v>
@@ -10677,7 +10677,7 @@
       </c>
       <c r="Z14" s="62"/>
     </row>
-    <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="71"/>
       <c r="B15" s="80" t="s">
         <v>165</v>
@@ -10723,7 +10723,7 @@
       </c>
       <c r="Z15" s="59"/>
     </row>
-    <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="69"/>
       <c r="B16" s="79" t="s">
         <v>166</v>
@@ -10769,7 +10769,7 @@
       </c>
       <c r="Z16" s="62"/>
     </row>
-    <row r="17" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="71"/>
       <c r="B17" s="80" t="s">
         <v>167</v>
@@ -10815,7 +10815,7 @@
       </c>
       <c r="Z17" s="59"/>
     </row>
-    <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="69"/>
       <c r="B18" s="79" t="s">
         <v>168</v>
@@ -10877,6 +10877,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2c089627-9960-44e1-9762-bfa3ba590a63">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D558A0C25AD9694BB62FFB42927C2A24" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd42f41f2bb46cd63a6e8ca5b25a11d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c089627-9960-44e1-9762-bfa3ba590a63" xmlns:ns3="64211953-cb0a-4a02-b1d5-47de0f0a68d5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd994a08d1fe56e517ba8eea0123f9e" ns2:_="" ns3:_="">
     <xsd:import namespace="2c089627-9960-44e1-9762-bfa3ba590a63"/>
@@ -11123,19 +11136,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="64211953-cb0a-4a02-b1d5-47de0f0a68d5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2c089627-9960-44e1-9762-bfa3ba590a63">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E72343A-1D3E-4810-AF97-187893FA4160}">
   <ds:schemaRefs>
@@ -11145,6 +11145,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D20332E-DAE9-4FA3-898D-66D0C67FC073}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="64211953-cb0a-4a02-b1d5-47de0f0a68d5"/>
+    <ds:schemaRef ds:uri="2c089627-9960-44e1-9762-bfa3ba590a63"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C868719-05F4-42CE-A730-B62E340093D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11161,15 +11172,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D20332E-DAE9-4FA3-898D-66D0C67FC073}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="64211953-cb0a-4a02-b1d5-47de0f0a68d5"/>
-    <ds:schemaRef ds:uri="2c089627-9960-44e1-9762-bfa3ba590a63"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>